<commit_message>
feat: update .gitignore and business strategy documents with new sections and formatting
</commit_message>
<xml_diff>
--- a/docs/bever_business_simulations.xlsx
+++ b/docs/bever_business_simulations.xlsx
@@ -93,13 +93,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$₦-C00]#,##0.00_);\([$₦-C00]#,##0.00\)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +126,6 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -581,158 +575,156 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1083,7 +1075,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1173,7 +1165,7 @@
       <c r="D2" s="1">
         <v>5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>4000</v>
       </c>
       <c r="F2" s="1">
@@ -1198,24 +1190,24 @@
         <f>F2*J2</f>
         <v>640000</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="1">
         <f>G2-(I2+K2)</f>
         <v>60000</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="1">
         <v>200000</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="1">
         <v>100000</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="1">
         <v>50000</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="1">
         <f>I2+K2+M2+N2+O2</f>
         <v>1090000</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="1">
         <f>G2-P2</f>
         <v>-290000</v>
       </c>
@@ -1224,58 +1216,58 @@
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>60</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>50</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>4000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f>C3*D3</f>
         <v>300</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <f>F3*E3</f>
         <v>1200000</v>
       </c>
       <c r="H3" s="1">
         <v>500</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>F3*H3</f>
         <v>150000</v>
       </c>
       <c r="J3" s="1">
         <v>3200</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <f>F3*J3</f>
         <v>960000</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <f>G3-(I3+K3)</f>
         <v>90000</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>200000</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>100000</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>50000</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <f>I3+K3+M3+N3+O3</f>
         <v>1460000</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <f>G3-P3</f>
         <v>-260000</v>
       </c>
@@ -1284,106 +1276,106 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>70</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>55</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>7</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>4200</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f>C4*D4</f>
         <v>385</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f>F4*E4</f>
         <v>1617000</v>
       </c>
       <c r="H4" s="1">
         <v>500</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f>F4*H4</f>
         <v>192500</v>
       </c>
       <c r="J4" s="1">
         <v>3200</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <f>F4*J4</f>
         <v>1232000</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <f>G4-(I4+K4)</f>
         <v>192500</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>200000</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>120000</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>60000</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <f>I4+K4+M4+N4+O4</f>
         <v>1804500</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="1">
         <f>G4-P4</f>
         <v>-187500</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="12:17">
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="12:17">
-      <c r="L7" s="4"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="12:17">
-      <c r="L8" s="4"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="12:17">
-      <c r="L9" s="4"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>